<commit_message>
Fix a lot of issues
</commit_message>
<xml_diff>
--- a/report_template/stylingReport.xlsx
+++ b/report_template/stylingReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>優</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,22 @@
   </si>
   <si>
     <t>不均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客戶編碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工廠代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顏色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺寸</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,25 +478,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.125" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="5.625" customWidth="1"/>
-    <col min="6" max="6" width="5.125" customWidth="1"/>
-    <col min="7" max="7" width="4.75" customWidth="1"/>
-    <col min="8" max="9" width="5.375" customWidth="1"/>
-    <col min="10" max="10" width="6.25" customWidth="1"/>
+    <col min="3" max="6" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="7.875" customWidth="1"/>
+    <col min="8" max="8" width="7.25" customWidth="1"/>
+    <col min="9" max="9" width="5.625" customWidth="1"/>
+    <col min="10" max="10" width="5.125" customWidth="1"/>
+    <col min="11" max="11" width="4.75" customWidth="1"/>
+    <col min="12" max="13" width="5.375" customWidth="1"/>
+    <col min="14" max="14" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -491,9 +509,13 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -501,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,24 +537,36 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>